<commit_message>
añadir reporte de resultado de apoyo
</commit_message>
<xml_diff>
--- a/core/reportes/bases/resultados-apoyo.xlsx
+++ b/core/reportes/bases/resultados-apoyo.xlsx
@@ -10,6 +10,9 @@
     <sheet name="Resumen y Datos Basicos" sheetId="31" state="hidden" r:id="rId1"/>
     <sheet name="Resultados" sheetId="6" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen y Datos Basicos'!$A$1:$F$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Resultados!$A$1:$U$26,Resultados!$A$28:$Y$64</definedName>
@@ -107,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
   <si>
     <t>Valoración</t>
   </si>
@@ -440,6 +443,21 @@
   </si>
   <si>
     <t>Nivel de revisión: 1</t>
+  </si>
+  <si>
+    <t>Necesidad de Formación</t>
+  </si>
+  <si>
+    <t>Tecno-Científica</t>
+  </si>
+  <si>
+    <t>Supervisoria Formativa</t>
+  </si>
+  <si>
+    <t>Técnica Administrativa y/o Apoyo</t>
+  </si>
+  <si>
+    <t>Seguridad Industrial</t>
   </si>
 </sst>
 </file>
@@ -1076,20 +1094,92 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1100,90 +1190,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1249,6 +1258,15 @@
     </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1306,62 +1324,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>33131</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>302315</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>127138</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="3 Flecha izquierda">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8086725" y="680831"/>
-          <a:ext cx="1311965" cy="284507"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="339966"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100"/>
-            <a:t>Ir al Inicio</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1383,7 +1345,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1407,6 +1369,55 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Resumen y Datos Basicos"/>
+      <sheetName val="Inicio"/>
+      <sheetName val="Pag 1 "/>
+      <sheetName val="Pag 2"/>
+      <sheetName val="Enc. Desempeño"/>
+      <sheetName val="Frec.y% Desempeño"/>
+      <sheetName val="Encuesta Comp.Tecnica"/>
+      <sheetName val="Frec.y% Comp.Tecnica"/>
+      <sheetName val="Encuesta Comp.Generica"/>
+      <sheetName val="Frec.y% Comp.Generica"/>
+      <sheetName val="Formación"/>
+      <sheetName val="Logros y Metas"/>
+      <sheetName val="Resultados"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>EVALUACIÓN DEL DESEMPEÑO</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Detección de Necesidades de Formación (DNF)</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2612,8 +2623,8 @@
   </sheetPr>
   <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2637,11 +2648,11 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:28" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2657,56 +2668,53 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="76"/>
-      <c r="U5" s="76"/>
+      <c r="A5" s="73" t="str">
+        <f>+'[1]Pag 1 '!B6</f>
+        <v>EVALUACIÓN DEL DESEMPEÑO</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
     </row>
     <row r="6" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="e">
-        <f>CONCATENATE("PERÍODO DE EVALUACIÓN ",+#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="72"/>
+      <c r="U6" s="72"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -2727,33 +2735,33 @@
       <c r="A8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="70" t="e">
+      <c r="B8" s="66" t="e">
         <f>+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="69" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="70" t="e">
+      <c r="Q8" s="65"/>
+      <c r="R8" s="66" t="e">
         <f>VLOOKUP(B8,'Resumen y Datos Basicos'!B1:F60,5,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="S8" s="71"/>
-      <c r="T8" s="72"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="68"/>
       <c r="AA8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2765,28 +2773,28 @@
       <c r="A9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="50" t="e">
+      <c r="B9" s="74" t="e">
         <f>VLOOKUP(B8,'Resumen y Datos Basicos'!B1:F60,3,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="52"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="76"/>
       <c r="AA9" s="6">
         <v>5</v>
       </c>
@@ -2808,31 +2816,31 @@
     </row>
     <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="73" t="s">
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="73" t="s">
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="75"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="70"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="71"/>
     </row>
     <row r="12" spans="1:28" ht="170.25" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -2898,82 +2906,25 @@
       <c r="A13" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!/20,#REF!/10)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!/20,#REF!/10)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!/20,#REF!/10)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!/20,#REF!/10)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F13" s="25" t="e">
-        <f>SUM(B13:E13)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K13" s="12" t="e">
-        <f>AVERAGE(G13:J13)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S13" s="11" t="e">
-        <f>IF($AA$9=5,#REF!,#REF!*2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T13" s="12" t="e">
-        <f>AVERAGE(L13:S13)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -3007,288 +2958,228 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="83"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="82" t="s">
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="84"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="81"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
     </row>
     <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
     </row>
     <row r="21" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
     </row>
     <row r="23" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="56" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="48"/>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="48"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
@@ -3306,84 +3197,83 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:24" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="88" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="90"/>
-      <c r="Q28" s="90"/>
-      <c r="R28" s="90"/>
-      <c r="S28" s="90"/>
-      <c r="T28" s="90"/>
-      <c r="U28" s="90"/>
-      <c r="V28" s="90"/>
-      <c r="W28" s="90"/>
-      <c r="X28" s="91"/>
+      <c r="A28" s="85" t="str">
+        <f>+[1]Formación!A13</f>
+        <v>Detección de Necesidades de Formación (DNF)</v>
+      </c>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="87"/>
+      <c r="Q28" s="87"/>
+      <c r="R28" s="87"/>
+      <c r="S28" s="87"/>
+      <c r="T28" s="87"/>
+      <c r="U28" s="87"/>
+      <c r="V28" s="87"/>
+      <c r="W28" s="87"/>
+      <c r="X28" s="88"/>
     </row>
     <row r="29" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="92" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B29" s="93"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="92" t="s">
+      <c r="A29" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="94"/>
-      <c r="G29" s="92" t="s">
+      <c r="F29" s="91"/>
+      <c r="G29" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="93"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="85" t="s">
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="N29" s="86"/>
-      <c r="O29" s="86"/>
-      <c r="P29" s="87"/>
-      <c r="Q29" s="86" t="s">
+      <c r="N29" s="83"/>
+      <c r="O29" s="83"/>
+      <c r="P29" s="84"/>
+      <c r="Q29" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="R29" s="86"/>
-      <c r="S29" s="86"/>
-      <c r="T29" s="86"/>
-      <c r="U29" s="86"/>
-      <c r="V29" s="86"/>
-      <c r="W29" s="86"/>
-      <c r="X29" s="87"/>
+      <c r="R29" s="83"/>
+      <c r="S29" s="83"/>
+      <c r="T29" s="83"/>
+      <c r="U29" s="83"/>
+      <c r="V29" s="83"/>
+      <c r="W29" s="83"/>
+      <c r="X29" s="84"/>
     </row>
     <row r="30" spans="1:24" ht="169.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="95"/>
-      <c r="B30" s="96"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="97"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96"/>
-      <c r="I30" s="96"/>
-      <c r="J30" s="96"/>
-      <c r="K30" s="96"/>
-      <c r="L30" s="96"/>
+      <c r="A30" s="92"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="93"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="93"/>
       <c r="M30" s="39" t="s">
         <v>14</v>
       </c>
@@ -3422,651 +3312,272 @@
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X31" s="38" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A31" s="52"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
+      <c r="S31" s="38"/>
+      <c r="T31" s="38"/>
+      <c r="U31" s="38"/>
+      <c r="V31" s="38"/>
+      <c r="W31" s="38"/>
+      <c r="X31" s="38"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X32" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X33" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X34" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A34" s="52"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
+      <c r="X34" s="22"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X35" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A35" s="52"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="22"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X36" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A36" s="52"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F37" s="49"/>
-      <c r="G37" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X37" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A37" s="52"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
+      <c r="X37" s="22"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F38" s="49"/>
-      <c r="G38" s="47" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X38" s="22" t="e">
-        <f>IF(#REF!&gt;0,+#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="22"/>
+      <c r="X38" s="22"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-      <c r="O39" s="61"/>
-      <c r="P39" s="61"/>
-      <c r="Q39" s="61"/>
-      <c r="R39" s="61"/>
-      <c r="S39" s="61"/>
-      <c r="T39" s="61"/>
-      <c r="U39" s="62"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="56"/>
+      <c r="T39" s="56"/>
+      <c r="U39" s="57"/>
     </row>
     <row r="40" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B40" s="10" t="e">
-        <f>COUNTIF(#REF!,A40)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A40" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
-      <c r="E40" s="10" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="E40" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
-      <c r="L40" s="10" t="e">
-        <f>COUNTIF(#REF!,E40)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M40" s="98" t="s">
+      <c r="L40" s="10"/>
+      <c r="M40" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="N40" s="98"/>
-      <c r="O40" s="98"/>
-      <c r="P40" s="98"/>
-      <c r="Q40" s="98"/>
-      <c r="R40" s="98"/>
-      <c r="S40" s="98"/>
-      <c r="T40" s="99"/>
-      <c r="U40" s="35" t="e">
-        <f>COUNTIF(#REF!,"&gt;=1")</f>
-        <v>#REF!</v>
-      </c>
+      <c r="N40" s="95"/>
+      <c r="O40" s="95"/>
+      <c r="P40" s="95"/>
+      <c r="Q40" s="95"/>
+      <c r="R40" s="95"/>
+      <c r="S40" s="95"/>
+      <c r="T40" s="96"/>
+      <c r="U40" s="35"/>
     </row>
     <row r="41" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B41" s="10" t="e">
-        <f>COUNTIF(#REF!,A41)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E41" s="10" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L41" s="10" t="e">
-        <f>COUNTIF(#REF!,E41)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A41" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="E41" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="L41" s="10"/>
     </row>
     <row r="42" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="10"/>
@@ -4078,269 +3589,238 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="100" t="s">
+      <c r="A43" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="101"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="101"/>
-      <c r="E43" s="101"/>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="101"/>
-      <c r="I43" s="101"/>
-      <c r="J43" s="101"/>
-      <c r="K43" s="101"/>
-      <c r="L43" s="101"/>
-      <c r="M43" s="101"/>
-      <c r="N43" s="101"/>
-      <c r="O43" s="102"/>
-      <c r="P43" s="63" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q43" s="64"/>
-      <c r="R43" s="64"/>
-      <c r="S43" s="65"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="98"/>
+      <c r="D43" s="98"/>
+      <c r="E43" s="98"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="98"/>
+      <c r="H43" s="98"/>
+      <c r="I43" s="98"/>
+      <c r="J43" s="98"/>
+      <c r="K43" s="98"/>
+      <c r="L43" s="98"/>
+      <c r="M43" s="98"/>
+      <c r="N43" s="98"/>
+      <c r="O43" s="99"/>
+      <c r="P43" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="59"/>
+      <c r="S43" s="60"/>
     </row>
     <row r="44" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="57" t="e">
+      <c r="A44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="61"/>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="63"/>
+    </row>
+    <row r="45" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="49"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="61"/>
+      <c r="Q45" s="62"/>
+      <c r="R45" s="62"/>
+      <c r="S45" s="63"/>
+    </row>
+    <row r="46" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="61"/>
+      <c r="Q46" s="62"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="63"/>
+    </row>
+    <row r="47" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="49"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="61"/>
+      <c r="Q47" s="62"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="63"/>
+    </row>
+    <row r="48" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="51"/>
+      <c r="P48" s="61"/>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="63"/>
+    </row>
+    <row r="49" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="49" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="58"/>
-      <c r="L44" s="58"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="58"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="66" t="e">
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="51"/>
+      <c r="P49" s="61" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="Q44" s="67"/>
-      <c r="R44" s="67"/>
-      <c r="S44" s="68"/>
-    </row>
-    <row r="45" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="e">
+      <c r="Q49" s="62"/>
+      <c r="R49" s="62"/>
+      <c r="S49" s="63"/>
+    </row>
+    <row r="50" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="49" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="59"/>
-      <c r="P45" s="66" t="e">
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="51"/>
+      <c r="P50" s="61" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="Q45" s="67"/>
-      <c r="R45" s="67"/>
-      <c r="S45" s="68"/>
-    </row>
-    <row r="46" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="57" t="e">
+      <c r="Q50" s="62"/>
+      <c r="R50" s="62"/>
+      <c r="S50" s="63"/>
+    </row>
+    <row r="51" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="49" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="59"/>
-      <c r="P46" s="66" t="e">
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="61" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="Q46" s="67"/>
-      <c r="R46" s="67"/>
-      <c r="S46" s="68"/>
-    </row>
-    <row r="47" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="59"/>
-      <c r="P47" s="66" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q47" s="67"/>
-      <c r="R47" s="67"/>
-      <c r="S47" s="68"/>
-    </row>
-    <row r="48" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="59"/>
-      <c r="P48" s="66" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q48" s="67"/>
-      <c r="R48" s="67"/>
-      <c r="S48" s="68"/>
-    </row>
-    <row r="49" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="57" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="59"/>
-      <c r="P49" s="66" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q49" s="67"/>
-      <c r="R49" s="67"/>
-      <c r="S49" s="68"/>
-    </row>
-    <row r="50" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="57" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="59"/>
-      <c r="P50" s="66" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q50" s="67"/>
-      <c r="R50" s="67"/>
-      <c r="S50" s="68"/>
-    </row>
-    <row r="51" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="57" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="59"/>
-      <c r="P51" s="66" t="e">
-        <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q51" s="67"/>
-      <c r="R51" s="67"/>
-      <c r="S51" s="68"/>
+      <c r="Q51" s="62"/>
+      <c r="R51" s="62"/>
+      <c r="S51" s="63"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="63" t="s">
+      <c r="A52" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
-      <c r="J52" s="64"/>
-      <c r="K52" s="64"/>
-      <c r="L52" s="64"/>
-      <c r="M52" s="64"/>
-      <c r="N52" s="64"/>
-      <c r="O52" s="64"/>
-      <c r="P52" s="64"/>
-      <c r="Q52" s="64"/>
-      <c r="R52" s="64"/>
-      <c r="S52" s="65"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="59"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="59"/>
+      <c r="M52" s="59"/>
+      <c r="N52" s="59"/>
+      <c r="O52" s="59"/>
+      <c r="P52" s="59"/>
+      <c r="Q52" s="59"/>
+      <c r="R52" s="59"/>
+      <c r="S52" s="60"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
@@ -4348,25 +3828,25 @@
       <c r="X52" s="1"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A53" s="78"/>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="79"/>
-      <c r="M53" s="79"/>
-      <c r="N53" s="79"/>
-      <c r="O53" s="79"/>
-      <c r="P53" s="79"/>
-      <c r="Q53" s="79"/>
-      <c r="R53" s="79"/>
-      <c r="S53" s="80"/>
+      <c r="A53" s="100"/>
+      <c r="B53" s="101"/>
+      <c r="C53" s="101"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="101"/>
+      <c r="F53" s="101"/>
+      <c r="G53" s="101"/>
+      <c r="H53" s="101"/>
+      <c r="I53" s="101"/>
+      <c r="J53" s="101"/>
+      <c r="K53" s="101"/>
+      <c r="L53" s="101"/>
+      <c r="M53" s="101"/>
+      <c r="N53" s="101"/>
+      <c r="O53" s="101"/>
+      <c r="P53" s="101"/>
+      <c r="Q53" s="101"/>
+      <c r="R53" s="101"/>
+      <c r="S53" s="102"/>
       <c r="T53" s="3"/>
       <c r="U53" s="8"/>
       <c r="V53" s="8"/>
@@ -4374,25 +3854,25 @@
       <c r="X53" s="1"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A54" s="78"/>
-      <c r="B54" s="79"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="79"/>
-      <c r="N54" s="79"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="79"/>
-      <c r="S54" s="80"/>
+      <c r="A54" s="100"/>
+      <c r="B54" s="101"/>
+      <c r="C54" s="101"/>
+      <c r="D54" s="101"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="101"/>
+      <c r="H54" s="101"/>
+      <c r="I54" s="101"/>
+      <c r="J54" s="101"/>
+      <c r="K54" s="101"/>
+      <c r="L54" s="101"/>
+      <c r="M54" s="101"/>
+      <c r="N54" s="101"/>
+      <c r="O54" s="101"/>
+      <c r="P54" s="101"/>
+      <c r="Q54" s="101"/>
+      <c r="R54" s="101"/>
+      <c r="S54" s="102"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
@@ -4400,25 +3880,25 @@
       <c r="X54" s="1"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A55" s="78"/>
-      <c r="B55" s="79"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="79"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
-      <c r="Q55" s="79"/>
-      <c r="R55" s="79"/>
-      <c r="S55" s="80"/>
+      <c r="A55" s="100"/>
+      <c r="B55" s="101"/>
+      <c r="C55" s="101"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="101"/>
+      <c r="F55" s="101"/>
+      <c r="G55" s="101"/>
+      <c r="H55" s="101"/>
+      <c r="I55" s="101"/>
+      <c r="J55" s="101"/>
+      <c r="K55" s="101"/>
+      <c r="L55" s="101"/>
+      <c r="M55" s="101"/>
+      <c r="N55" s="101"/>
+      <c r="O55" s="101"/>
+      <c r="P55" s="101"/>
+      <c r="Q55" s="101"/>
+      <c r="R55" s="101"/>
+      <c r="S55" s="102"/>
       <c r="T55" s="3"/>
       <c r="U55" s="8"/>
       <c r="V55" s="8"/>
@@ -4426,25 +3906,25 @@
       <c r="X55" s="1"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A56" s="66"/>
-      <c r="B56" s="67"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="67"/>
-      <c r="E56" s="67"/>
-      <c r="F56" s="67"/>
-      <c r="G56" s="67"/>
-      <c r="H56" s="67"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="67"/>
-      <c r="K56" s="67"/>
-      <c r="L56" s="67"/>
-      <c r="M56" s="67"/>
-      <c r="N56" s="67"/>
-      <c r="O56" s="67"/>
-      <c r="P56" s="67"/>
-      <c r="Q56" s="67"/>
-      <c r="R56" s="67"/>
-      <c r="S56" s="68"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="50"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="50"/>
+      <c r="S56" s="51"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
@@ -4481,15 +3961,15 @@
       <c r="A58" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="81" t="s">
+      <c r="D58" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="E58" s="81"/>
-      <c r="F58" s="81"/>
-      <c r="G58" s="81"/>
-      <c r="H58" s="81"/>
-      <c r="I58" s="81"/>
-      <c r="J58" s="81"/>
+      <c r="E58" s="78"/>
+      <c r="F58" s="78"/>
+      <c r="G58" s="78"/>
+      <c r="H58" s="78"/>
+      <c r="I58" s="78"/>
+      <c r="J58" s="78"/>
       <c r="M58" s="26"/>
       <c r="N58" s="26"/>
       <c r="O58" s="26"/>
@@ -4843,12 +4323,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100526F55E509A791499B5FB50D930526F2" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="69fc4eb0c2ce4169b40c10b57224ba8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ebba8a198e9bb40c3eeca6d0bd41257a">
     <xsd:element name="properties">
@@ -4962,7 +4436,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4971,16 +4445,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4C85B0F-1DCF-44D3-BFBD-56B7901BCE44}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CF53B1C-6A51-40EA-BAF7-6C3B831D3D53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4996,10 +4467,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B2A4B8D-1F51-4D98-A7C2-EC11EE68F57E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4C85B0F-1DCF-44D3-BFBD-56B7901BCE44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
añadir mensajes de feedback
</commit_message>
<xml_diff>
--- a/core/reportes/bases/resultados-apoyo.xlsx
+++ b/core/reportes/bases/resultados-apoyo.xlsx
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="117">
   <si>
     <t>Valoración</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>Seguridad Industrial</t>
+  </si>
+  <si>
+    <t>EVALUACIÓN DEL DESEMPEÑO</t>
   </si>
 </sst>
 </file>
@@ -1094,6 +1097,60 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1103,26 +1160,107 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1132,141 +1270,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2623,8 +2626,8 @@
   </sheetPr>
   <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:S56"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2648,11 +2651,11 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:28" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2668,53 +2671,52 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="str">
-        <f>+'[1]Pag 1 '!B6</f>
-        <v>EVALUACIÓN DEL DESEMPEÑO</v>
-      </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
+      <c r="A5" s="96" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="96"/>
+      <c r="S5" s="96"/>
+      <c r="T5" s="96"/>
+      <c r="U5" s="96"/>
     </row>
     <row r="6" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="72"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="72"/>
+      <c r="A6" s="95"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -2735,33 +2737,33 @@
       <c r="A8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="66" t="e">
+      <c r="B8" s="89" t="e">
         <f>+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="65" t="s">
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="66" t="e">
+      <c r="Q8" s="88"/>
+      <c r="R8" s="89" t="e">
         <f>VLOOKUP(B8,'Resumen y Datos Basicos'!B1:F60,5,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="S8" s="67"/>
-      <c r="T8" s="68"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="91"/>
       <c r="AA8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2773,28 +2775,28 @@
       <c r="A9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="74" t="e">
+      <c r="B9" s="97" t="e">
         <f>VLOOKUP(B8,'Resumen y Datos Basicos'!B1:F60,3,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="76"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="98"/>
+      <c r="P9" s="98"/>
+      <c r="Q9" s="98"/>
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="99"/>
       <c r="AA9" s="6">
         <v>5</v>
       </c>
@@ -2816,31 +2818,31 @@
     </row>
     <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="69" t="s">
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="69" t="s">
+      <c r="H11" s="93"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="70"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="70"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="71"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="93"/>
+      <c r="P11" s="93"/>
+      <c r="Q11" s="93"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="93"/>
+      <c r="T11" s="94"/>
     </row>
     <row r="12" spans="1:28" ht="170.25" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -2958,228 +2960,228 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="80"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="79" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="78"/>
+      <c r="P16" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="Q16" s="80"/>
-      <c r="R16" s="81"/>
+      <c r="Q16" s="77"/>
+      <c r="R16" s="78"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
     </row>
     <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
     </row>
     <row r="21" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="48"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="62"/>
     </row>
     <row r="23" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="48"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="62"/>
+      <c r="R24" s="62"/>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="48"/>
-      <c r="R25" s="48"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="48"/>
-      <c r="R26" s="48"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="62"/>
+      <c r="R26" s="62"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
@@ -3197,83 +3199,83 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:24" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="85" t="str">
+      <c r="A28" s="66" t="str">
         <f>+[1]Formación!A13</f>
         <v>Detección de Necesidades de Formación (DNF)</v>
       </c>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
-      <c r="L28" s="86"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="87"/>
-      <c r="O28" s="87"/>
-      <c r="P28" s="87"/>
-      <c r="Q28" s="87"/>
-      <c r="R28" s="87"/>
-      <c r="S28" s="87"/>
-      <c r="T28" s="87"/>
-      <c r="U28" s="87"/>
-      <c r="V28" s="87"/>
-      <c r="W28" s="87"/>
-      <c r="X28" s="88"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="68"/>
+      <c r="Q28" s="68"/>
+      <c r="R28" s="68"/>
+      <c r="S28" s="68"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="68"/>
+      <c r="V28" s="68"/>
+      <c r="W28" s="68"/>
+      <c r="X28" s="69"/>
     </row>
     <row r="29" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="89" t="s">
+      <c r="A29" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="90"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="89" t="s">
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="91"/>
-      <c r="G29" s="89" t="s">
+      <c r="F29" s="72"/>
+      <c r="G29" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="82" t="s">
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="N29" s="83"/>
-      <c r="O29" s="83"/>
-      <c r="P29" s="84"/>
-      <c r="Q29" s="83" t="s">
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="R29" s="83"/>
-      <c r="S29" s="83"/>
-      <c r="T29" s="83"/>
-      <c r="U29" s="83"/>
-      <c r="V29" s="83"/>
-      <c r="W29" s="83"/>
-      <c r="X29" s="84"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="60"/>
+      <c r="T29" s="60"/>
+      <c r="U29" s="60"/>
+      <c r="V29" s="60"/>
+      <c r="W29" s="60"/>
+      <c r="X29" s="61"/>
     </row>
     <row r="30" spans="1:24" ht="169.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="92"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="92"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="93"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
       <c r="M30" s="39" t="s">
         <v>14</v>
       </c>
@@ -3312,18 +3314,18 @@
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="54"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="51"/>
       <c r="M31" s="38"/>
       <c r="N31" s="38"/>
       <c r="O31" s="38"/>
@@ -3338,18 +3340,18 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="54"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="51"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -3364,18 +3366,18 @@
       <c r="X32" s="22"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="54"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="51"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -3390,18 +3392,18 @@
       <c r="X33" s="22"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="54"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="51"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -3416,18 +3418,18 @@
       <c r="X34" s="22"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="54"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="51"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -3442,18 +3444,18 @@
       <c r="X35" s="22"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="54"/>
+      <c r="A36" s="50"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="51"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -3468,18 +3470,18 @@
       <c r="X36" s="22"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="54"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="51"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -3494,18 +3496,18 @@
       <c r="X37" s="22"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="54"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="51"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -3520,29 +3522,29 @@
       <c r="X38" s="22"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
-      <c r="T39" s="56"/>
-      <c r="U39" s="57"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="101"/>
+      <c r="H39" s="101"/>
+      <c r="I39" s="101"/>
+      <c r="J39" s="101"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="101"/>
+      <c r="M39" s="101"/>
+      <c r="N39" s="101"/>
+      <c r="O39" s="101"/>
+      <c r="P39" s="101"/>
+      <c r="Q39" s="101"/>
+      <c r="R39" s="101"/>
+      <c r="S39" s="101"/>
+      <c r="T39" s="101"/>
+      <c r="U39" s="102"/>
     </row>
     <row r="40" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
@@ -3557,16 +3559,16 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="L40" s="10"/>
-      <c r="M40" s="95" t="s">
+      <c r="M40" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="N40" s="95"/>
-      <c r="O40" s="95"/>
-      <c r="P40" s="95"/>
-      <c r="Q40" s="95"/>
-      <c r="R40" s="95"/>
-      <c r="S40" s="95"/>
-      <c r="T40" s="96"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="46"/>
       <c r="U40" s="35"/>
     </row>
     <row r="41" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3589,238 +3591,238 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="98"/>
-      <c r="I43" s="98"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="99"/>
-      <c r="P43" s="58" t="s">
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="Q43" s="59"/>
-      <c r="R43" s="59"/>
-      <c r="S43" s="60"/>
+      <c r="Q43" s="81"/>
+      <c r="R43" s="81"/>
+      <c r="S43" s="82"/>
     </row>
     <row r="44" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="50"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="61"/>
-      <c r="Q44" s="62"/>
-      <c r="R44" s="62"/>
-      <c r="S44" s="63"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="54"/>
+      <c r="P44" s="47"/>
+      <c r="Q44" s="48"/>
+      <c r="R44" s="48"/>
+      <c r="S44" s="49"/>
     </row>
     <row r="45" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="51"/>
-      <c r="P45" s="61"/>
-      <c r="Q45" s="62"/>
-      <c r="R45" s="62"/>
-      <c r="S45" s="63"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53"/>
+      <c r="O45" s="54"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="48"/>
+      <c r="R45" s="48"/>
+      <c r="S45" s="49"/>
     </row>
     <row r="46" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="51"/>
-      <c r="P46" s="61"/>
-      <c r="Q46" s="62"/>
-      <c r="R46" s="62"/>
-      <c r="S46" s="63"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="53"/>
+      <c r="M46" s="53"/>
+      <c r="N46" s="53"/>
+      <c r="O46" s="54"/>
+      <c r="P46" s="47"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
+      <c r="S46" s="49"/>
     </row>
     <row r="47" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-      <c r="L47" s="50"/>
-      <c r="M47" s="50"/>
-      <c r="N47" s="50"/>
-      <c r="O47" s="51"/>
-      <c r="P47" s="61"/>
-      <c r="Q47" s="62"/>
-      <c r="R47" s="62"/>
-      <c r="S47" s="63"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+      <c r="L47" s="53"/>
+      <c r="M47" s="53"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="54"/>
+      <c r="P47" s="47"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="48"/>
+      <c r="S47" s="49"/>
     </row>
     <row r="48" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="49"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
-      <c r="M48" s="50"/>
-      <c r="N48" s="50"/>
-      <c r="O48" s="51"/>
-      <c r="P48" s="61"/>
-      <c r="Q48" s="62"/>
-      <c r="R48" s="62"/>
-      <c r="S48" s="63"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="54"/>
+      <c r="P48" s="47"/>
+      <c r="Q48" s="48"/>
+      <c r="R48" s="48"/>
+      <c r="S48" s="49"/>
     </row>
     <row r="49" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="e">
+      <c r="A49" s="52" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="50"/>
-      <c r="M49" s="50"/>
-      <c r="N49" s="50"/>
-      <c r="O49" s="51"/>
-      <c r="P49" s="61" t="e">
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="53"/>
+      <c r="N49" s="53"/>
+      <c r="O49" s="54"/>
+      <c r="P49" s="47" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="Q49" s="62"/>
-      <c r="R49" s="62"/>
-      <c r="S49" s="63"/>
+      <c r="Q49" s="48"/>
+      <c r="R49" s="48"/>
+      <c r="S49" s="49"/>
     </row>
     <row r="50" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="e">
+      <c r="A50" s="52" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="50"/>
-      <c r="M50" s="50"/>
-      <c r="N50" s="50"/>
-      <c r="O50" s="51"/>
-      <c r="P50" s="61" t="e">
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="53"/>
+      <c r="N50" s="53"/>
+      <c r="O50" s="54"/>
+      <c r="P50" s="47" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="Q50" s="62"/>
-      <c r="R50" s="62"/>
-      <c r="S50" s="63"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="49"/>
     </row>
     <row r="51" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="e">
+      <c r="A51" s="52" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="50"/>
-      <c r="M51" s="50"/>
-      <c r="N51" s="50"/>
-      <c r="O51" s="51"/>
-      <c r="P51" s="61" t="e">
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="53"/>
+      <c r="L51" s="53"/>
+      <c r="M51" s="53"/>
+      <c r="N51" s="53"/>
+      <c r="O51" s="54"/>
+      <c r="P51" s="47" t="e">
         <f>+IF(#REF!&lt;&gt;"",#REF!,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="Q51" s="62"/>
-      <c r="R51" s="62"/>
-      <c r="S51" s="63"/>
+      <c r="Q51" s="48"/>
+      <c r="R51" s="48"/>
+      <c r="S51" s="49"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="58" t="s">
+      <c r="A52" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="59"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="59"/>
-      <c r="M52" s="59"/>
-      <c r="N52" s="59"/>
-      <c r="O52" s="59"/>
-      <c r="P52" s="59"/>
-      <c r="Q52" s="59"/>
-      <c r="R52" s="59"/>
-      <c r="S52" s="60"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="81"/>
+      <c r="J52" s="81"/>
+      <c r="K52" s="81"/>
+      <c r="L52" s="81"/>
+      <c r="M52" s="81"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="81"/>
+      <c r="P52" s="81"/>
+      <c r="Q52" s="81"/>
+      <c r="R52" s="81"/>
+      <c r="S52" s="82"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
@@ -3828,25 +3830,25 @@
       <c r="X52" s="1"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A53" s="100"/>
-      <c r="B53" s="101"/>
-      <c r="C53" s="101"/>
-      <c r="D53" s="101"/>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101"/>
-      <c r="G53" s="101"/>
-      <c r="H53" s="101"/>
-      <c r="I53" s="101"/>
-      <c r="J53" s="101"/>
-      <c r="K53" s="101"/>
-      <c r="L53" s="101"/>
-      <c r="M53" s="101"/>
-      <c r="N53" s="101"/>
-      <c r="O53" s="101"/>
-      <c r="P53" s="101"/>
-      <c r="Q53" s="101"/>
-      <c r="R53" s="101"/>
-      <c r="S53" s="102"/>
+      <c r="A53" s="83"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="84"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="84"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="84"/>
+      <c r="N53" s="84"/>
+      <c r="O53" s="84"/>
+      <c r="P53" s="84"/>
+      <c r="Q53" s="84"/>
+      <c r="R53" s="84"/>
+      <c r="S53" s="85"/>
       <c r="T53" s="3"/>
       <c r="U53" s="8"/>
       <c r="V53" s="8"/>
@@ -3854,25 +3856,25 @@
       <c r="X53" s="1"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A54" s="100"/>
-      <c r="B54" s="101"/>
-      <c r="C54" s="101"/>
-      <c r="D54" s="101"/>
-      <c r="E54" s="101"/>
-      <c r="F54" s="101"/>
-      <c r="G54" s="101"/>
-      <c r="H54" s="101"/>
-      <c r="I54" s="101"/>
-      <c r="J54" s="101"/>
-      <c r="K54" s="101"/>
-      <c r="L54" s="101"/>
-      <c r="M54" s="101"/>
-      <c r="N54" s="101"/>
-      <c r="O54" s="101"/>
-      <c r="P54" s="101"/>
-      <c r="Q54" s="101"/>
-      <c r="R54" s="101"/>
-      <c r="S54" s="102"/>
+      <c r="A54" s="83"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="84"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="84"/>
+      <c r="M54" s="84"/>
+      <c r="N54" s="84"/>
+      <c r="O54" s="84"/>
+      <c r="P54" s="84"/>
+      <c r="Q54" s="84"/>
+      <c r="R54" s="84"/>
+      <c r="S54" s="85"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
@@ -3880,25 +3882,25 @@
       <c r="X54" s="1"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A55" s="100"/>
-      <c r="B55" s="101"/>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="101"/>
-      <c r="F55" s="101"/>
-      <c r="G55" s="101"/>
-      <c r="H55" s="101"/>
-      <c r="I55" s="101"/>
-      <c r="J55" s="101"/>
-      <c r="K55" s="101"/>
-      <c r="L55" s="101"/>
-      <c r="M55" s="101"/>
-      <c r="N55" s="101"/>
-      <c r="O55" s="101"/>
-      <c r="P55" s="101"/>
-      <c r="Q55" s="101"/>
-      <c r="R55" s="101"/>
-      <c r="S55" s="102"/>
+      <c r="A55" s="83"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="84"/>
+      <c r="G55" s="84"/>
+      <c r="H55" s="84"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="84"/>
+      <c r="K55" s="84"/>
+      <c r="L55" s="84"/>
+      <c r="M55" s="84"/>
+      <c r="N55" s="84"/>
+      <c r="O55" s="84"/>
+      <c r="P55" s="84"/>
+      <c r="Q55" s="84"/>
+      <c r="R55" s="84"/>
+      <c r="S55" s="85"/>
       <c r="T55" s="3"/>
       <c r="U55" s="8"/>
       <c r="V55" s="8"/>
@@ -3906,25 +3908,25 @@
       <c r="X55" s="1"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A56" s="49"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="50"/>
-      <c r="L56" s="50"/>
-      <c r="M56" s="50"/>
-      <c r="N56" s="50"/>
-      <c r="O56" s="50"/>
-      <c r="P56" s="50"/>
-      <c r="Q56" s="50"/>
-      <c r="R56" s="50"/>
-      <c r="S56" s="51"/>
+      <c r="A56" s="52"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="53"/>
+      <c r="M56" s="53"/>
+      <c r="N56" s="53"/>
+      <c r="O56" s="53"/>
+      <c r="P56" s="53"/>
+      <c r="Q56" s="53"/>
+      <c r="R56" s="53"/>
+      <c r="S56" s="54"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
@@ -3961,15 +3963,15 @@
       <c r="A58" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="78" t="s">
+      <c r="D58" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="E58" s="78"/>
-      <c r="F58" s="78"/>
-      <c r="G58" s="78"/>
-      <c r="H58" s="78"/>
-      <c r="I58" s="78"/>
-      <c r="J58" s="78"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="86"/>
+      <c r="H58" s="86"/>
+      <c r="I58" s="86"/>
+      <c r="J58" s="86"/>
       <c r="M58" s="26"/>
       <c r="N58" s="26"/>
       <c r="O58" s="26"/>
@@ -3994,13 +3996,13 @@
       <c r="X59" s="1"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D60" s="77"/>
-      <c r="E60" s="77"/>
-      <c r="F60" s="77"/>
-      <c r="G60" s="77"/>
-      <c r="H60" s="77"/>
-      <c r="I60" s="77"/>
-      <c r="J60" s="77"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="79"/>
+      <c r="F60" s="79"/>
+      <c r="G60" s="79"/>
+      <c r="H60" s="79"/>
+      <c r="I60" s="79"/>
+      <c r="J60" s="79"/>
       <c r="M60" s="26"/>
       <c r="N60" s="26"/>
       <c r="O60" s="26"/>
@@ -4218,79 +4220,6 @@
     <sortCondition ref="M56:M115"/>
   </sortState>
   <mergeCells count="89">
-    <mergeCell ref="M40:T40"/>
-    <mergeCell ref="P50:S50"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="P46:S46"/>
-    <mergeCell ref="P47:S47"/>
-    <mergeCell ref="A47:O47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A45:O45"/>
-    <mergeCell ref="A46:O46"/>
-    <mergeCell ref="A43:O43"/>
-    <mergeCell ref="P45:S45"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:L37"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="A25:O25"/>
-    <mergeCell ref="Q29:X29"/>
-    <mergeCell ref="A28:X28"/>
-    <mergeCell ref="A29:D30"/>
-    <mergeCell ref="E29:F30"/>
-    <mergeCell ref="G29:L30"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="A22:O22"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="A17:O17"/>
-    <mergeCell ref="A18:O18"/>
-    <mergeCell ref="A16:O16"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="A20:O20"/>
-    <mergeCell ref="A21:O21"/>
-    <mergeCell ref="D60:J60"/>
-    <mergeCell ref="A52:S52"/>
-    <mergeCell ref="A53:S53"/>
-    <mergeCell ref="A54:S54"/>
-    <mergeCell ref="A55:S55"/>
-    <mergeCell ref="A56:S56"/>
-    <mergeCell ref="D58:J58"/>
-    <mergeCell ref="P51:S51"/>
-    <mergeCell ref="P48:S48"/>
-    <mergeCell ref="P49:S49"/>
-    <mergeCell ref="A51:O51"/>
-    <mergeCell ref="A48:O48"/>
-    <mergeCell ref="A49:O49"/>
-    <mergeCell ref="A50:O50"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:L34"/>
-    <mergeCell ref="G35:L35"/>
-    <mergeCell ref="G36:L36"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B8:O8"/>
-    <mergeCell ref="A6:U6"/>
-    <mergeCell ref="A5:U5"/>
-    <mergeCell ref="B9:T9"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:T11"/>
     <mergeCell ref="A23:O23"/>
     <mergeCell ref="P23:R23"/>
     <mergeCell ref="A44:O44"/>
@@ -4307,6 +4236,79 @@
     <mergeCell ref="P44:S44"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="G31:L31"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B8:O8"/>
+    <mergeCell ref="A6:U6"/>
+    <mergeCell ref="A5:U5"/>
+    <mergeCell ref="B9:T9"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="L11:T11"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="G35:L35"/>
+    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="P51:S51"/>
+    <mergeCell ref="P48:S48"/>
+    <mergeCell ref="P49:S49"/>
+    <mergeCell ref="A51:O51"/>
+    <mergeCell ref="A48:O48"/>
+    <mergeCell ref="A49:O49"/>
+    <mergeCell ref="A50:O50"/>
+    <mergeCell ref="D60:J60"/>
+    <mergeCell ref="A52:S52"/>
+    <mergeCell ref="A53:S53"/>
+    <mergeCell ref="A54:S54"/>
+    <mergeCell ref="A55:S55"/>
+    <mergeCell ref="A56:S56"/>
+    <mergeCell ref="D58:J58"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="A22:O22"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="A17:O17"/>
+    <mergeCell ref="A18:O18"/>
+    <mergeCell ref="A16:O16"/>
+    <mergeCell ref="A19:O19"/>
+    <mergeCell ref="A20:O20"/>
+    <mergeCell ref="A21:O21"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="A25:O25"/>
+    <mergeCell ref="Q29:X29"/>
+    <mergeCell ref="A28:X28"/>
+    <mergeCell ref="A29:D30"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="G29:L30"/>
+    <mergeCell ref="M40:T40"/>
+    <mergeCell ref="P50:S50"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="P46:S46"/>
+    <mergeCell ref="P47:S47"/>
+    <mergeCell ref="A47:O47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A45:O45"/>
+    <mergeCell ref="A46:O46"/>
+    <mergeCell ref="A43:O43"/>
+    <mergeCell ref="P45:S45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:L37"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -4437,18 +4439,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4468,18 +4470,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B2A4B8D-1F51-4D98-A7C2-EC11EE68F57E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4C85B0F-1DCF-44D3-BFBD-56B7901BCE44}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B2A4B8D-1F51-4D98-A7C2-EC11EE68F57E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>